<commit_message>
Limit early retirement just for existing ICEs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Add_FOM.xlsx
+++ b/SuppXLS/Scen_TRA_Add_FOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48185994-C83B-4DC0-9720-A04A4C8F7996}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC7798A-8A1D-478B-AD78-A99D509238FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -422,13 +422,13 @@
     <t>other_indexes</t>
   </si>
   <si>
-    <t>*Existing*</t>
-  </si>
-  <si>
-    <t>T-CAR-*</t>
-  </si>
-  <si>
     <t>NCAP_FOM</t>
+  </si>
+  <si>
+    <t>T-CAR-ICE*</t>
+  </si>
+  <si>
+    <t>*Existing</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1023,40 +1023,40 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="7" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" style="7" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="7"/>
+    <col min="29" max="29" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C3" s="8" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -1170,12 +1170,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>45</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>48</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>49</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>50</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>52</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>53</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>54</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>55</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>56</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>57</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>59</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>60</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>61</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>62</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>63</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>64</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>65</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>66</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>67</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>68</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>69</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>70</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>71</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>72</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>75</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>76</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>77</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>78</v>
       </c>
@@ -1766,7 +1766,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1786,37 +1786,37 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK5" sqref="AK5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="33" width="10.7109375" customWidth="1"/>
-    <col min="34" max="34" width="10.7109375" style="7" customWidth="1"/>
-    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="33" width="10.6640625" customWidth="1"/>
+    <col min="34" max="34" width="10.6640625" style="7" customWidth="1"/>
+    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1830,7 +1830,7 @@
       <c r="AP2" s="3"/>
       <c r="AQ2" s="3"/>
     </row>
-    <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1985,9 +1985,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H4" s="14">
         <v>2</v>
@@ -2074,10 +2074,10 @@
         <v>81</v>
       </c>
       <c r="AK4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
@@ -2107,7 +2107,7 @@
       <c r="AJ5" s="14"/>
       <c r="AK5" s="14"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -2118,7 +2118,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -2129,7 +2129,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -2140,7 +2140,7 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -2151,7 +2151,7 @@
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -2162,7 +2162,7 @@
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -2173,7 +2173,7 @@
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -2199,30 +2199,30 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="34" width="10.7109375" customWidth="1"/>
-    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="34" width="10.6640625" customWidth="1"/>
+    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2235,7 +2235,7 @@
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
     </row>
-    <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Modify fixed O&M costs for early retirement
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Add_FOM.xlsx
+++ b/SuppXLS/Scen_TRA_Add_FOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC7798A-8A1D-478B-AD78-A99D509238FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58993029-78A1-4B9E-BBC7-3E1B5E88FEC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -1786,15 +1786,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK5" sqref="AK5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -1841,7 +1841,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>15</v>
@@ -1989,86 +1989,89 @@
       <c r="D4" t="s">
         <v>80</v>
       </c>
+      <c r="E4">
+        <v>2018</v>
+      </c>
       <c r="H4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ4" t="s">
         <v>81</v>
@@ -2078,34 +2081,188 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
+      <c r="E5">
+        <v>2020</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0</v>
+      </c>
+      <c r="O5" s="14">
+        <v>0</v>
+      </c>
+      <c r="P5" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+      <c r="R5" s="14">
+        <v>0</v>
+      </c>
+      <c r="S5" s="14">
+        <v>0</v>
+      </c>
+      <c r="T5" s="14">
+        <v>0</v>
+      </c>
+      <c r="U5" s="14">
+        <v>0</v>
+      </c>
+      <c r="V5" s="14">
+        <v>0</v>
+      </c>
+      <c r="W5" s="14">
+        <v>0</v>
+      </c>
+      <c r="X5" s="14">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK5" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>2025</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
+        <v>1</v>
+      </c>
+      <c r="K6" s="14">
+        <v>1</v>
+      </c>
+      <c r="L6" s="14">
+        <v>1</v>
+      </c>
+      <c r="M6" s="14">
+        <v>1</v>
+      </c>
+      <c r="N6" s="14">
+        <v>1</v>
+      </c>
+      <c r="O6" s="14">
+        <v>1</v>
+      </c>
+      <c r="P6" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>1</v>
+      </c>
+      <c r="R6" s="14">
+        <v>1</v>
+      </c>
+      <c r="S6" s="14">
+        <v>1</v>
+      </c>
+      <c r="T6" s="14">
+        <v>1</v>
+      </c>
+      <c r="U6" s="14">
+        <v>1</v>
+      </c>
+      <c r="V6" s="14">
+        <v>1</v>
+      </c>
+      <c r="W6" s="14">
+        <v>1</v>
+      </c>
+      <c r="X6" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK6" s="14" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C11" s="14"/>

</xml_diff>

<commit_message>
Modify FOM for early retirement
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Add_FOM.xlsx
+++ b/SuppXLS/Scen_TRA_Add_FOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58993029-78A1-4B9E-BBC7-3E1B5E88FEC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF863B04-0F28-4FB2-A4CC-0D478B3EE06F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -1787,7 +1787,7 @@
   <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2081,6 +2081,9 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="D5" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="E5">
         <v>2020</v>
       </c>
@@ -2173,6 +2176,9 @@
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="D6" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="E6">
         <v>2025</v>
       </c>

</xml_diff>

<commit_message>
Modify Fixed O&M for early retirement
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Add_FOM.xlsx
+++ b/SuppXLS/Scen_TRA_Add_FOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF863B04-0F28-4FB2-A4CC-0D478B3EE06F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7944662B-97D5-4217-8CE2-CF403BBE026A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -1786,8 +1786,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG17" sqref="AG17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,89 +1989,86 @@
       <c r="D4" t="s">
         <v>80</v>
       </c>
-      <c r="E4">
-        <v>2018</v>
-      </c>
       <c r="H4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4" t="s">
         <v>81</v>
@@ -2081,194 +2078,66 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="D5" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5">
-        <v>2020</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="14">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14">
-        <v>0</v>
-      </c>
-      <c r="K5" s="14">
-        <v>0</v>
-      </c>
-      <c r="L5" s="14">
-        <v>0</v>
-      </c>
-      <c r="M5" s="14">
-        <v>0</v>
-      </c>
-      <c r="N5" s="14">
-        <v>0</v>
-      </c>
-      <c r="O5" s="14">
-        <v>0</v>
-      </c>
-      <c r="P5" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="14">
-        <v>0</v>
-      </c>
-      <c r="R5" s="14">
-        <v>0</v>
-      </c>
-      <c r="S5" s="14">
-        <v>0</v>
-      </c>
-      <c r="T5" s="14">
-        <v>0</v>
-      </c>
-      <c r="U5" s="14">
-        <v>0</v>
-      </c>
-      <c r="V5" s="14">
-        <v>0</v>
-      </c>
-      <c r="W5" s="14">
-        <v>0</v>
-      </c>
-      <c r="X5" s="14">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK5" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="D5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="14"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="D6" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6">
-        <v>2025</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="14">
-        <v>1</v>
-      </c>
-      <c r="K6" s="14">
-        <v>1</v>
-      </c>
-      <c r="L6" s="14">
-        <v>1</v>
-      </c>
-      <c r="M6" s="14">
-        <v>1</v>
-      </c>
-      <c r="N6" s="14">
-        <v>1</v>
-      </c>
-      <c r="O6" s="14">
-        <v>1</v>
-      </c>
-      <c r="P6" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="14">
-        <v>1</v>
-      </c>
-      <c r="R6" s="14">
-        <v>1</v>
-      </c>
-      <c r="S6" s="14">
-        <v>1</v>
-      </c>
-      <c r="T6" s="14">
-        <v>1</v>
-      </c>
-      <c r="U6" s="14">
-        <v>1</v>
-      </c>
-      <c r="V6" s="14">
-        <v>1</v>
-      </c>
-      <c r="W6" s="14">
-        <v>1</v>
-      </c>
-      <c r="X6" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="14">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK6" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="D6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="14"/>
+      <c r="AH6" s="14"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="14"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C11" s="14"/>

</xml_diff>